<commit_message>
Rework get data algorithms to support multifrequency and horizontal series. Now all the 7 test cases are passing with parameters!!
</commit_message>
<xml_diff>
--- a/tests/integration_cases/expected/test_case7.xlsx
+++ b/tests/integration_cases/expected/test_case7.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-2026" yWindow="-76" windowWidth="8538" windowHeight="6448" tabRatio="601"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="601"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -34,88 +39,88 @@
     <t>datetime</t>
   </si>
   <si>
-    <t>Current Account - Goods (7)</t>
-  </si>
-  <si>
-    <t>Current Account - Goods (7) - Exports FOB</t>
-  </si>
-  <si>
-    <t>Current Account - Goods (7) - Imports FOB</t>
-  </si>
-  <si>
-    <t>Current Account - Services</t>
-  </si>
-  <si>
-    <t>Current Account - Services - Exports</t>
-  </si>
-  <si>
-    <t>Current Account - Services - Imports</t>
-  </si>
-  <si>
-    <t>Current Account - Income</t>
-  </si>
-  <si>
-    <t>Current Account - Income - Investment income</t>
-  </si>
-  <si>
-    <t>Current Account - Income - Investment income - Interests</t>
-  </si>
-  <si>
-    <t>Current Account - Income - Investment income - Interests - Credit</t>
-  </si>
-  <si>
-    <t>Current Account - Income - Investment income - Interests - Debit</t>
-  </si>
-  <si>
-    <t>Current Account - Income - Investment income - Profits and dividends</t>
-  </si>
-  <si>
-    <t>Current Account - Income - Investment income - Profits and dividends - Credit</t>
-  </si>
-  <si>
-    <t>Current Account - Income - Investment income - Profits and dividends - Debit</t>
-  </si>
-  <si>
-    <t>Current Account - Income - Other Income</t>
-  </si>
-  <si>
-    <t>Current Account - Current Transfers</t>
-  </si>
-  <si>
-    <t>Capital and Financial Account - Capital Account</t>
-  </si>
-  <si>
-    <t>Capital and Financial Account - Financial Account</t>
-  </si>
-  <si>
-    <t>Capital and Financial Account - Financial Account - Banking Sector</t>
-  </si>
-  <si>
-    <t>Capital and Financial Account - Financial Account - Banking Sector - Central Bank</t>
-  </si>
-  <si>
-    <t>Capital and Financial Account - Financial Account - Banking Sector - Other financial entities</t>
-  </si>
-  <si>
-    <t>Capital and Financial Account - Financial Account - Nonfinancial Public Sector</t>
-  </si>
-  <si>
-    <t>Capital and Financial Account - Financial Account - Nonfinancial Public Sector - National Government (5) (6)</t>
-  </si>
-  <si>
-    <t>Capital and Financial Account - Financial Account - Nonfinancial Public Sector - Local Governments</t>
-  </si>
-  <si>
-    <t>Capital and Financial Account - Financial Account - Nonfinancial Public Sector - Companies and other</t>
-  </si>
-  <si>
-    <t>Capital and Financial Account - Financial Account - Nonfinancial Private Sector</t>
-  </si>
-  <si>
-    <t>International Reserves Variation - BCRA International Reserves</t>
-  </si>
-  <si>
-    <t>International Reserves Variation - Exchange rate adjustment</t>
+    <t>Goods (7)</t>
+  </si>
+  <si>
+    <t>Exports FOB</t>
+  </si>
+  <si>
+    <t>Imports FOB</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Exports</t>
+  </si>
+  <si>
+    <t>Imports</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Investment income</t>
+  </si>
+  <si>
+    <t>Interests</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Debit</t>
+  </si>
+  <si>
+    <t>Profits and dividends</t>
+  </si>
+  <si>
+    <t>Other Income</t>
+  </si>
+  <si>
+    <t>Current Transfers</t>
+  </si>
+  <si>
+    <t>Capital Account</t>
+  </si>
+  <si>
+    <t>Financial Account</t>
+  </si>
+  <si>
+    <t>Banking Sector</t>
+  </si>
+  <si>
+    <t>Central Bank</t>
+  </si>
+  <si>
+    <t>Other financial entities</t>
+  </si>
+  <si>
+    <t>Nonfinancial Public Sector</t>
+  </si>
+  <si>
+    <t>National Government (5) (6)</t>
+  </si>
+  <si>
+    <t>Local Governments</t>
+  </si>
+  <si>
+    <t>Companies and other</t>
+  </si>
+  <si>
+    <t>Nonfinancial Private Sector</t>
+  </si>
+  <si>
+    <t>BCRA International Reserves</t>
+  </si>
+  <si>
+    <t>Exchange rate adjustment</t>
+  </si>
+  <si>
+    <t>Credit.2</t>
+  </si>
+  <si>
+    <t>Debit.2</t>
   </si>
 </sst>
 </file>
@@ -123,10 +128,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="_ [$€-2]\ * #,##0.00_ ;_ [$€-2]\ * \-#,##0.00_ ;_ [$€-2]\ * &quot;-&quot;??_ "/>
-    <numFmt numFmtId="166" formatCode="#,##0.00_);\(#,##0.00\);&quot; --- &quot;"/>
+    <numFmt numFmtId="164" formatCode="_ [$€-2]\ * #,##0.00_ ;_ [$€-2]\ * \-#,##0.00_ ;_ [$€-2]\ * &quot;-&quot;??_ "/>
+    <numFmt numFmtId="165" formatCode="#,##0.00_);\(#,##0.00\);&quot; --- &quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -140,6 +145,18 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,10 +176,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -172,8 +203,22 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="17">
     <cellStyle name="Euro" xfId="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Nulos" xfId="2"/>
   </cellStyles>
@@ -542,18 +587,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH24"/>
+  <dimension ref="A1:AH23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.5546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="3" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" s="3" customFormat="1" ht="24">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -597,49 +642,49 @@
         <v>17</v>
       </c>
       <c r="O1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="S1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="T1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="AD1" s="3" t="s">
         <v>2</v>
@@ -648,16 +693,16 @@
         <v>3</v>
       </c>
       <c r="AF1" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AG1" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="AH1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34">
       <c r="A2" s="1">
         <v>33604</v>
       </c>
@@ -761,7 +806,7 @@
         <v>14981.7</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34">
       <c r="A3" s="1">
         <v>33970</v>
       </c>
@@ -865,7 +910,7 @@
         <v>16872.3</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34">
       <c r="A4" s="1">
         <v>34335</v>
       </c>
@@ -969,7 +1014,7 @@
         <v>21675.1</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34">
       <c r="A5" s="1">
         <v>34700</v>
       </c>
@@ -1073,7 +1118,7 @@
         <v>20199.7</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34">
       <c r="A6" s="1">
         <v>35065</v>
       </c>
@@ -1177,7 +1222,7 @@
         <v>23855.1</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34">
       <c r="A7" s="1">
         <v>35431</v>
       </c>
@@ -1281,7 +1326,7 @@
         <v>30450.2</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34">
       <c r="A8" s="1">
         <v>35796</v>
       </c>
@@ -1385,7 +1430,7 @@
         <v>31377.4</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34">
       <c r="A9" s="1">
         <v>36161</v>
       </c>
@@ -1489,7 +1534,7 @@
         <v>25508.2</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34">
       <c r="A10" s="1">
         <v>36526</v>
       </c>
@@ -1593,7 +1638,7 @@
         <v>25280.5</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34">
       <c r="A11" s="1">
         <v>36892</v>
       </c>
@@ -1697,7 +1742,7 @@
         <v>20319.599999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34">
       <c r="A12" s="1">
         <v>37257</v>
       </c>
@@ -1801,7 +1846,7 @@
         <v>8989.5</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34">
       <c r="A13" s="1">
         <v>37622</v>
       </c>
@@ -1905,7 +1950,7 @@
         <v>13850.8</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34">
       <c r="A14" s="1">
         <v>37987</v>
       </c>
@@ -2009,7 +2054,7 @@
         <v>22445.3</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34">
       <c r="A15" s="1">
         <v>38353</v>
       </c>
@@ -2113,7 +2158,7 @@
         <v>28686.94</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34">
       <c r="A16" s="1">
         <v>38718</v>
       </c>
@@ -2217,7 +2262,7 @@
         <v>34153.699999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34">
       <c r="A17" s="1">
         <v>39083</v>
       </c>
@@ -2321,7 +2366,7 @@
         <v>44707.5</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34">
       <c r="A18" s="1">
         <v>39448</v>
       </c>
@@ -2425,7 +2470,7 @@
         <v>57462.5</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34">
       <c r="A19" s="1">
         <v>39814</v>
       </c>
@@ -2529,7 +2574,7 @@
         <v>38786.267</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34">
       <c r="A20" s="1">
         <v>40179</v>
       </c>
@@ -2633,7 +2678,7 @@
         <v>56792.578073999997</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34">
       <c r="A21" s="1">
         <v>40544</v>
       </c>
@@ -2737,7 +2782,7 @@
         <v>74319.348503179994</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34">
       <c r="A22" s="1">
         <v>40909</v>
       </c>
@@ -2841,7 +2886,7 @@
         <v>68020.282609000002</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34">
       <c r="A23" s="1">
         <v>41275</v>
       </c>
@@ -2944,11 +2989,13 @@
       <c r="AH23" s="2">
         <v>73655.53667300001</v>
       </c>
-    </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>